<commit_message>
Aggiunto risultati in .gitignore
</commit_message>
<xml_diff>
--- a/risultati/performance_model.xlsx
+++ b/risultati/performance_model.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,18 +436,34 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Valore</t>
+          <t>Exp 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Exp 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Exp 3</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Accuracy</t>
+          <t>Specificity</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9512195121951219</v>
+        <v>0.9692307692307692</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9503546099290781</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9777777777777777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sistemate le docstring e i commenti delle istruzioni
</commit_message>
<xml_diff>
--- a/risultati/performance_model.xlsx
+++ b/risultati/performance_model.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.967479674796748</v>
+        <v>0.9611273080660837</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.03252032520325199</v>
+        <v>0.03887269193391642</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.9459459459459459</v>
+        <v>0.852891156462585</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.9767441860465116</v>
+        <v>0.9704081632653061</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.961221724170324</v>
+        <v>0.8537029040016562</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiunti mock interfaccia ai tests
</commit_message>
<xml_diff>
--- a/risultati/performance_model.xlsx
+++ b/risultati/performance_model.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,26 +444,18 @@
           <t>Exp 2</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Exp 3</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>Specificity</t>
+          <t>Error Rate</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9692307692307692</v>
+        <v>0.05691056910569103</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9503546099290781</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.9777777777777777</v>
+        <v>0.02439024390243905</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornate tutte le DocString delle classi e dei metodi che erano dipendenti da interfaccia_utente, mancavano i parametri di ingresso relativi all'input
</commit_message>
<xml_diff>
--- a/risultati/performance_model.xlsx
+++ b/risultati/performance_model.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,17 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Valore</t>
+          <t>Exp 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Exp 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Exp 3</t>
         </is>
       </c>
     </row>
@@ -447,27 +457,77 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.983739837398374</v>
+        <v>0.9707317073170731</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9609756097560975</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9512195121951219</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Sensitivity</t>
+          <t>Error Rate</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9761904761904762</v>
+        <v>0.02926829268292686</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.03902439024390247</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.04878048780487809</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>Sensitivity</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.9436619718309859</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.9354838709677419</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.9342105263157895</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
           <t>Specificity</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0.9876543209876543</v>
+      <c r="B5" t="n">
+        <v>0.9850746268656716</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.972027972027972</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.9612403100775194</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Geometric Mean</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9641459769084411</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.9535808775146716</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.9476290497834435</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit prima di pullare dal main remoto
</commit_message>
<xml_diff>
--- a/risultati/performance_model.xlsx
+++ b/risultati/performance_model.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,27 +447,47 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.983739837398374</v>
+        <v>0.9701149425287354</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Sensitivity</t>
+          <t>Error Rate</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.9761904761904762</v>
+        <v>0.02988505747126437</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
+          <t>Sensitivity</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.9451013922518159</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
           <t>Specificity</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>0.9876543209876543</v>
+      <c r="B5" t="n">
+        <v>0.9840499920124092</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>Geometric Mean</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.9643111674053102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato il file README
</commit_message>
<xml_diff>
--- a/risultati/performance_model.xlsx
+++ b/risultati/performance_model.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,27 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Valore</t>
+          <t>Exp 1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Exp 2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Exp 3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Exp 4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Exp 5</t>
         </is>
       </c>
     </row>
@@ -447,47 +467,63 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.9396551724137931</v>
+        <v>0.9635036496350365</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9854014598540146</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.9854014598540146</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.9343065693430657</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9708029197080292</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>Error Rate</t>
+          <t>Sensitivity</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.06034482758620685</v>
+        <v>0.9387755102040817</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.8837209302325582</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9574468085106383</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>Sensitivity</t>
+          <t>Geometric Mean</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.8611111111111112</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Specificity</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>0.975</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>Geometric Mean</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.916287800493564</v>
+        <v>0.9578307278188505</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.9881652636251156</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0.983192080250175</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.9198455219574726</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9675588936937934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>